<commit_message>
excel data driven module push 2
</commit_message>
<xml_diff>
--- a/Signupusers.xlsx
+++ b/Signupusers.xlsx
@@ -427,7 +427,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -487,7 +487,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>raj12212@mail.com</t>
+          <t>raj001@mail.com</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>taj12322@mail.com</t>
+          <t>taj002@mail.com</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>gani12311@bhai.com</t>
+          <t>gani003@bhai.com</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">

</xml_diff>